<commit_message>
update master jasa harga bertingkat
</commit_message>
<xml_diff>
--- a/ImportExport/ExcelFiles/MasterJasaHargaBertingkat.xlsx
+++ b/ImportExport/ExcelFiles/MasterJasaHargaBertingkat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohyusufz\Desktop\Axata\AxataPOSFilesResources-main\ImportExport\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFB80A3-2DC2-46AD-BDBE-DB2066C95AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDE99CA-8026-44F4-B513-664B9C53EF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>SATUAN</t>
   </si>
   <si>
     <t>HARGAJUAL</t>
-  </si>
-  <si>
-    <t>JMLBARANG</t>
   </si>
   <si>
     <t>JML1</t>
@@ -81,7 +78,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,12 +106,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,7 +145,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -164,16 +155,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -451,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -464,25 +452,24 @@
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -493,63 +480,57 @@
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2">
         <v>1000</v>
       </c>
       <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>900</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <v>800</v>
+      </c>
+      <c r="J2">
         <v>100</v>
       </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>900</v>
-      </c>
-      <c r="I2">
-        <v>50</v>
-      </c>
-      <c r="J2">
-        <v>800</v>
-      </c>
       <c r="K2">
-        <v>100</v>
-      </c>
-      <c r="L2">
         <v>750</v>
       </c>
     </row>

</xml_diff>